<commit_message>
used nano sec instead of milli sec for unique number
</commit_message>
<xml_diff>
--- a/Resources/dsrProfileDataTemp.xlsx
+++ b/Resources/dsrProfileDataTemp.xlsx
@@ -144,40 +144,40 @@
     <t>Hassam DSR OB</t>
   </si>
   <si>
-    <t>AUTODSR_3B8FF</t>
-  </si>
-  <si>
-    <t>Father_A6</t>
-  </si>
-  <si>
-    <t>03979108725</t>
-  </si>
-  <si>
-    <t>EMP00128E</t>
-  </si>
-  <si>
-    <t>AUTODSR_BF349</t>
-  </si>
-  <si>
-    <t>Father_0E</t>
-  </si>
-  <si>
-    <t>03979108729</t>
-  </si>
-  <si>
-    <t>EMP54D935</t>
-  </si>
-  <si>
-    <t>AUTODSR_6583A</t>
-  </si>
-  <si>
-    <t>Father_DE</t>
-  </si>
-  <si>
-    <t>03979108732</t>
-  </si>
-  <si>
-    <t>EMP71D447</t>
+    <t>AUTODSR_735C4</t>
+  </si>
+  <si>
+    <t>Father_557C</t>
+  </si>
+  <si>
+    <t>03303184100</t>
+  </si>
+  <si>
+    <t>EMP5A21C3</t>
+  </si>
+  <si>
+    <t>AUTODSR_68BEB</t>
+  </si>
+  <si>
+    <t>Father_9B3A</t>
+  </si>
+  <si>
+    <t>03305402500</t>
+  </si>
+  <si>
+    <t>EMP5C5B75</t>
+  </si>
+  <si>
+    <t>AUTODSR_1204D</t>
+  </si>
+  <si>
+    <t>Father_A820</t>
+  </si>
+  <si>
+    <t>03307303800</t>
+  </si>
+  <si>
+    <t>EMP211591</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
data source from excel instead of json
</commit_message>
<xml_diff>
--- a/Resources/dsrProfileDataTemp.xlsx
+++ b/Resources/dsrProfileDataTemp.xlsx
@@ -144,40 +144,40 @@
     <t>Hassam DSR OB</t>
   </si>
   <si>
-    <t>AUTODSR_0EC0E</t>
-  </si>
-  <si>
-    <t>Father_78D5</t>
-  </si>
-  <si>
-    <t>03072833300</t>
-  </si>
-  <si>
-    <t>EMPC92E58</t>
-  </si>
-  <si>
-    <t>AUTODSR_8032D</t>
-  </si>
-  <si>
-    <t>Father_1381</t>
-  </si>
-  <si>
-    <t>03078799100</t>
-  </si>
-  <si>
-    <t>EMP67B6C4</t>
-  </si>
-  <si>
-    <t>AUTODSR_FA1B4</t>
-  </si>
-  <si>
-    <t>Father_D1E4</t>
-  </si>
-  <si>
-    <t>03083543800</t>
-  </si>
-  <si>
-    <t>EMP5BAB29</t>
+    <t>AUTODSR_33662</t>
+  </si>
+  <si>
+    <t>Father_D0A9</t>
+  </si>
+  <si>
+    <t>03851754800</t>
+  </si>
+  <si>
+    <t>EMPDD7C41</t>
+  </si>
+  <si>
+    <t>AUTODSR_FC2B2</t>
+  </si>
+  <si>
+    <t>Father_6326</t>
+  </si>
+  <si>
+    <t>03854217700</t>
+  </si>
+  <si>
+    <t>EMP7A5A9E</t>
+  </si>
+  <si>
+    <t>AUTODSR_B0763</t>
+  </si>
+  <si>
+    <t>Father_B318</t>
+  </si>
+  <si>
+    <t>03855535900</t>
+  </si>
+  <si>
+    <t>EMP706899</t>
   </si>
 </sst>
 </file>

</xml_diff>